<commit_message>
updated 114 yelp zips
</commit_message>
<xml_diff>
--- a/YelpOverallRating.xlsx
+++ b/YelpOverallRating.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>restaurantCount</t>
   </si>
@@ -58,6 +58,12 @@
     <t>15005</t>
   </si>
   <si>
+    <t>15006</t>
+  </si>
+  <si>
+    <t>15007</t>
+  </si>
+  <si>
     <t>15102</t>
   </si>
   <si>
@@ -67,9 +73,15 @@
     <t>15104</t>
   </si>
   <si>
+    <t>15015</t>
+  </si>
+  <si>
     <t>15017</t>
   </si>
   <si>
+    <t>15018</t>
+  </si>
+  <si>
     <t>15020</t>
   </si>
   <si>
@@ -88,6 +100,9 @@
     <t>15108</t>
   </si>
   <si>
+    <t>15028</t>
+  </si>
+  <si>
     <t>15030</t>
   </si>
   <si>
@@ -97,6 +112,9 @@
     <t>15031</t>
   </si>
   <si>
+    <t>15034</t>
+  </si>
+  <si>
     <t>15110</t>
   </si>
   <si>
@@ -121,12 +139,21 @@
     <t>15116</t>
   </si>
   <si>
+    <t>15047</t>
+  </si>
+  <si>
+    <t>15049</t>
+  </si>
+  <si>
     <t>15120</t>
   </si>
   <si>
     <t>15126</t>
   </si>
   <si>
+    <t>15051</t>
+  </si>
+  <si>
     <t>15642</t>
   </si>
   <si>
@@ -160,6 +187,9 @@
     <t>15146</t>
   </si>
   <si>
+    <t>15064</t>
+  </si>
+  <si>
     <t>15668</t>
   </si>
   <si>
@@ -178,6 +208,9 @@
     <t>15139</t>
   </si>
   <si>
+    <t>15140</t>
+  </si>
+  <si>
     <t>15201</t>
   </si>
   <si>
@@ -187,6 +220,9 @@
     <t>15203</t>
   </si>
   <si>
+    <t>15204</t>
+  </si>
+  <si>
     <t>15205</t>
   </si>
   <si>
@@ -287,6 +323,18 @@
   </si>
   <si>
     <t>15241</t>
+  </si>
+  <si>
+    <t>15243</t>
+  </si>
+  <si>
+    <t>15260</t>
+  </si>
+  <si>
+    <t>15290</t>
+  </si>
+  <si>
+    <t>15142</t>
   </si>
   <si>
     <t>15075</t>
@@ -698,7 +746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -849,34 +897,16 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1.964285714285714</v>
-      </c>
-      <c r="D5">
-        <v>3.681818181818182</v>
-      </c>
-      <c r="E5">
-        <v>2.823051948051948</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>3.125</v>
-      </c>
-      <c r="H5">
-        <v>1.9625</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>9</v>
-      </c>
-      <c r="J5">
-        <v>3.166666666666667</v>
-      </c>
-      <c r="K5">
-        <v>3.383333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -884,25 +914,13 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1.25</v>
-      </c>
-      <c r="D6">
-        <v>3.333333333333333</v>
-      </c>
-      <c r="E6">
-        <v>2.291666666666667</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>3.75</v>
-      </c>
-      <c r="H6">
-        <v>2.075</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -913,28 +931,34 @@
         <v>16</v>
       </c>
       <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1.964285714285714</v>
+      </c>
+      <c r="D7">
+        <v>3.681818181818182</v>
+      </c>
+      <c r="E7">
+        <v>2.823051948051948</v>
+      </c>
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>1.25</v>
-      </c>
-      <c r="D7">
-        <v>4.231988472622478</v>
-      </c>
-      <c r="E7">
-        <v>2.740994236311239</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
       <c r="G7">
-        <v>4.5</v>
+        <v>3.125</v>
       </c>
       <c r="H7">
-        <v>2.55</v>
+        <v>1.9625</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <v>3.166666666666667</v>
+      </c>
+      <c r="K7">
+        <v>3.383333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -942,34 +966,28 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="D8">
-        <v>3.298</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="E8">
-        <v>2.649</v>
+        <v>2.291666666666667</v>
       </c>
       <c r="F8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>3.333333333333333</v>
+        <v>3.75</v>
       </c>
       <c r="H8">
-        <v>2.566666666666667</v>
+        <v>2.075</v>
       </c>
       <c r="I8">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <v>3.1</v>
-      </c>
-      <c r="K8">
-        <v>2.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -977,25 +995,25 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>1.25</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>4.231988472622478</v>
       </c>
       <c r="E9">
-        <v>3.125</v>
+        <v>2.740994236311239</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="H9">
-        <v>2.6</v>
+        <v>2.55</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1006,34 +1024,16 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>2.25</v>
-      </c>
-      <c r="D10">
-        <v>4.119349005424954</v>
-      </c>
-      <c r="E10">
-        <v>3.184674502712477</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>3.611111111111111</v>
-      </c>
-      <c r="H10">
-        <v>2.705555555555556</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>3.785714285714286</v>
-      </c>
-      <c r="K10">
-        <v>3.292857142857143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1041,22 +1041,34 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>6.25</v>
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3.298</v>
+      </c>
+      <c r="E11">
+        <v>2.649</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>3.5</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="H11">
-        <v>2.05</v>
+        <v>2.566666666666667</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>3.1</v>
+      </c>
+      <c r="K11">
+        <v>2.55</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1064,25 +1076,13 @@
         <v>21</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1.25</v>
-      </c>
-      <c r="D12">
-        <v>3.213114754098361</v>
-      </c>
-      <c r="E12">
-        <v>2.23155737704918</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>3.5</v>
-      </c>
-      <c r="H12">
-        <v>1.95</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1093,28 +1093,28 @@
         <v>22</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1.25</v>
       </c>
       <c r="D13">
-        <v>3.137931034482758</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>2.193965517241379</v>
+        <v>3.125</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>2.6</v>
       </c>
       <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>4</v>
-      </c>
-      <c r="K13">
-        <v>2.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1122,34 +1122,34 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>1.964285714285714</v>
+        <v>2.25</v>
       </c>
       <c r="D14">
-        <v>3.818345323741007</v>
+        <v>4.119349005424954</v>
       </c>
       <c r="E14">
-        <v>2.891315519013361</v>
+        <v>3.184674502712477</v>
       </c>
       <c r="F14">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>3.433333333333333</v>
+        <v>3.611111111111111</v>
       </c>
       <c r="H14">
-        <v>3.216666666666667</v>
+        <v>2.705555555555556</v>
       </c>
       <c r="I14">
         <v>7</v>
       </c>
       <c r="J14">
-        <v>3.5</v>
+        <v>3.785714285714286</v>
       </c>
       <c r="K14">
-        <v>3.15</v>
+        <v>3.292857142857143</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1157,19 +1157,19 @@
         <v>24</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1.25</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>2.625</v>
+        <v>6.25</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>3.5</v>
+      </c>
+      <c r="H15">
+        <v>2.05</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1180,25 +1180,25 @@
         <v>25</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>1.25</v>
       </c>
       <c r="D16">
-        <v>3.5</v>
+        <v>3.213114754098361</v>
       </c>
       <c r="E16">
-        <v>2.375</v>
+        <v>2.23155737704918</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
         <v>3.5</v>
       </c>
       <c r="H16">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1209,28 +1209,28 @@
         <v>26</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>1.25</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>3.137931034482758</v>
       </c>
       <c r="E17">
-        <v>2.125</v>
+        <v>2.193965517241379</v>
       </c>
       <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>2.5</v>
-      </c>
-      <c r="H17">
-        <v>1.45</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>2.2</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1238,34 +1238,34 @@
         <v>27</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C18">
-        <v>1.25</v>
+        <v>1.964285714285714</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>3.818345323741007</v>
       </c>
       <c r="E18">
-        <v>1.125</v>
+        <v>2.891315519013361</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>3.433333333333333</v>
       </c>
       <c r="H18">
-        <v>0.6</v>
+        <v>3.216666666666667</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="K18">
-        <v>0.7</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1273,16 +1273,10 @@
         <v>28</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1.25</v>
-      </c>
-      <c r="D19">
-        <v>4.5</v>
-      </c>
-      <c r="E19">
-        <v>2.875</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1308,22 +1302,10 @@
         <v>2.625</v>
       </c>
       <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>3.25</v>
-      </c>
-      <c r="H20">
-        <v>1.825</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>4</v>
-      </c>
-      <c r="K20">
-        <v>2.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1331,34 +1313,28 @@
         <v>30</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>1.25</v>
       </c>
       <c r="D21">
-        <v>3.605633802816901</v>
+        <v>3.5</v>
       </c>
       <c r="E21">
-        <v>2.427816901408451</v>
+        <v>2.375</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="H21">
-        <v>2.15</v>
+        <v>1.85</v>
       </c>
       <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>4.25</v>
-      </c>
-      <c r="K21">
-        <v>2.525</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1366,34 +1342,28 @@
         <v>31</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>1.25</v>
       </c>
       <c r="D22">
-        <v>3.166666666666667</v>
+        <v>3</v>
       </c>
       <c r="E22">
-        <v>2.208333333333333</v>
+        <v>2.125</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>2.333333333333333</v>
+        <v>2.5</v>
       </c>
       <c r="H22">
-        <v>1.466666666666667</v>
+        <v>1.45</v>
       </c>
       <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22">
-        <v>3.75</v>
-      </c>
-      <c r="K22">
-        <v>2.275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1401,34 +1371,22 @@
         <v>32</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>1.634615384615384</v>
-      </c>
-      <c r="D23">
-        <v>3.405511811023622</v>
-      </c>
-      <c r="E23">
-        <v>2.520063597819503</v>
+        <v>6.25</v>
       </c>
       <c r="F23">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>3.55</v>
+        <v>2.5</v>
       </c>
       <c r="H23">
-        <v>2.775</v>
+        <v>1.35</v>
       </c>
       <c r="I23">
-        <v>8</v>
-      </c>
-      <c r="J23">
-        <v>3.5</v>
-      </c>
-      <c r="K23">
-        <v>3.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1442,16 +1400,28 @@
         <v>1.25</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>2.625</v>
+        <v>1.125</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.6</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1459,34 +1429,22 @@
         <v>34</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>2.083333333333333</v>
+        <v>1.25</v>
       </c>
       <c r="D25">
-        <v>3.922535211267606</v>
+        <v>4.5</v>
       </c>
       <c r="E25">
-        <v>3.002934272300469</v>
+        <v>2.875</v>
       </c>
       <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25">
-        <v>3.75</v>
-      </c>
-      <c r="H25">
-        <v>2.075</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>3.5</v>
-      </c>
-      <c r="K25">
-        <v>1.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1494,34 +1452,34 @@
         <v>35</v>
       </c>
       <c r="B26">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>1.964285714285714</v>
+        <v>1.25</v>
       </c>
       <c r="D26">
-        <v>3.200308505949758</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>2.582297110117736</v>
+        <v>2.625</v>
       </c>
       <c r="F26">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>3.642857142857143</v>
+        <v>3.25</v>
       </c>
       <c r="H26">
-        <v>3.921428571428572</v>
+        <v>1.825</v>
       </c>
       <c r="I26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>3.833333333333333</v>
+        <v>4</v>
       </c>
       <c r="K26">
-        <v>2.516666666666667</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1529,34 +1487,34 @@
         <v>36</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C27">
         <v>1.25</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>3.605633802816901</v>
       </c>
       <c r="E27">
-        <v>2.625</v>
+        <v>2.427816901408451</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="H27">
-        <v>2.1</v>
+        <v>2.15</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>4.25</v>
       </c>
       <c r="K27">
-        <v>0.7</v>
+        <v>2.525</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1564,34 +1522,34 @@
         <v>37</v>
       </c>
       <c r="B28">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>1.75</v>
+        <v>1.25</v>
       </c>
       <c r="D28">
-        <v>3.481641468682505</v>
+        <v>3.166666666666667</v>
       </c>
       <c r="E28">
-        <v>2.615820734341253</v>
+        <v>2.208333333333333</v>
       </c>
       <c r="F28">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G28">
-        <v>3.571428571428572</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="H28">
-        <v>2.485714285714286</v>
+        <v>1.466666666666667</v>
       </c>
       <c r="I28">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J28">
-        <v>3.714285714285714</v>
+        <v>3.75</v>
       </c>
       <c r="K28">
-        <v>3.257142857142857</v>
+        <v>2.275</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1599,34 +1557,34 @@
         <v>38</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>3.75</v>
+        <v>1.634615384615384</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>3.405511811023622</v>
       </c>
       <c r="E29">
-        <v>3.875</v>
+        <v>2.520063597819503</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G29">
-        <v>4.5</v>
+        <v>3.55</v>
       </c>
       <c r="H29">
-        <v>2.45</v>
+        <v>2.775</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J29">
-        <v>1.25</v>
+        <v>3.5</v>
       </c>
       <c r="K29">
-        <v>1.025</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1634,34 +1592,22 @@
         <v>39</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>2.083333333333333</v>
+        <v>1.25</v>
       </c>
       <c r="D30">
-        <v>3.701637666325486</v>
+        <v>4</v>
       </c>
       <c r="E30">
-        <v>2.89248549982941</v>
+        <v>2.625</v>
       </c>
       <c r="F30">
-        <v>5</v>
-      </c>
-      <c r="G30">
-        <v>3.4</v>
-      </c>
-      <c r="H30">
-        <v>2.2</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="J30">
-        <v>2.5</v>
-      </c>
-      <c r="K30">
-        <v>1.65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1669,16 +1615,16 @@
         <v>40</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>1.25</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="D31">
-        <v>3.857142857142857</v>
+        <v>3.922535211267606</v>
       </c>
       <c r="E31">
-        <v>2.553571428571429</v>
+        <v>3.002934272300469</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -1690,13 +1636,13 @@
         <v>2.075</v>
       </c>
       <c r="I31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J31">
-        <v>3.833333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="K31">
-        <v>2.516666666666667</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1704,34 +1650,16 @@
         <v>41</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>2.159090909090909</v>
-      </c>
-      <c r="D32">
-        <v>3.855828220858896</v>
-      </c>
-      <c r="E32">
-        <v>3.007459564974902</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>7</v>
-      </c>
-      <c r="G32">
-        <v>4.285714285714286</v>
-      </c>
-      <c r="H32">
-        <v>2.842857142857143</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>3</v>
-      </c>
-      <c r="J32">
-        <v>2.666666666666667</v>
-      </c>
-      <c r="K32">
-        <v>1.933333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1739,34 +1667,16 @@
         <v>42</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>1.25</v>
-      </c>
-      <c r="D33">
-        <v>3.433962264150944</v>
-      </c>
-      <c r="E33">
-        <v>2.341981132075472</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>2</v>
-      </c>
-      <c r="G33">
-        <v>2.75</v>
-      </c>
-      <c r="H33">
-        <v>1.575</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>2</v>
-      </c>
-      <c r="J33">
-        <v>3.5</v>
-      </c>
-      <c r="K33">
-        <v>2.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1774,34 +1684,34 @@
         <v>43</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>1.25</v>
+        <v>1.964285714285714</v>
       </c>
       <c r="D34">
-        <v>3.142857142857143</v>
+        <v>3.201232937032144</v>
       </c>
       <c r="E34">
-        <v>2.196428571428571</v>
+        <v>2.582759325658929</v>
       </c>
       <c r="F34">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G34">
-        <v>3.625</v>
+        <v>3.642857142857143</v>
       </c>
       <c r="H34">
-        <v>2.2125</v>
+        <v>3.921428571428572</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>3.833333333333333</v>
       </c>
       <c r="K34">
-        <v>0.7</v>
+        <v>2.516666666666667</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1809,28 +1719,34 @@
         <v>44</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>1.25</v>
       </c>
       <c r="D35">
-        <v>4.25</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>2.75</v>
+        <v>2.625</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="H35">
-        <v>2.45</v>
+        <v>2.1</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>0.7</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1838,34 +1754,16 @@
         <v>45</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>1.25</v>
-      </c>
-      <c r="D36">
-        <v>3.409090909090909</v>
-      </c>
-      <c r="E36">
-        <v>2.329545454545455</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>2.5</v>
-      </c>
-      <c r="H36">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36">
-        <v>4</v>
-      </c>
-      <c r="K36">
-        <v>2.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1873,34 +1771,34 @@
         <v>46</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="D37">
-        <v>3.566666666666667</v>
+        <v>3.481641468682505</v>
       </c>
       <c r="E37">
-        <v>2.408333333333333</v>
+        <v>2.615820734341253</v>
       </c>
       <c r="F37">
         <v>7</v>
       </c>
       <c r="G37">
-        <v>4.5</v>
+        <v>3.571428571428572</v>
       </c>
       <c r="H37">
-        <v>2.95</v>
+        <v>2.485714285714286</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J37">
-        <v>2.333333333333333</v>
+        <v>3.714285714285714</v>
       </c>
       <c r="K37">
-        <v>1.766666666666667</v>
+        <v>3.257142857142857</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1908,34 +1806,34 @@
         <v>47</v>
       </c>
       <c r="B38">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>3.107142857142857</v>
+        <v>3.75</v>
       </c>
       <c r="D38">
-        <v>3.559947643979057</v>
+        <v>4</v>
       </c>
       <c r="E38">
-        <v>3.333545250560957</v>
+        <v>3.875</v>
       </c>
       <c r="F38">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G38">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="H38">
-        <v>2.95</v>
+        <v>2.45</v>
       </c>
       <c r="I38">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J38">
-        <v>3.75</v>
+        <v>1.25</v>
       </c>
       <c r="K38">
-        <v>4.275</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1943,34 +1841,34 @@
         <v>48</v>
       </c>
       <c r="B39">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>2.583333333333333</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="D39">
-        <v>3.766260162601626</v>
+        <v>3.701637666325486</v>
       </c>
       <c r="E39">
-        <v>3.17479674796748</v>
+        <v>2.89248549982941</v>
       </c>
       <c r="F39">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G39">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="H39">
-        <v>2.45</v>
+        <v>2.2</v>
       </c>
       <c r="I39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J39">
         <v>2.5</v>
       </c>
       <c r="K39">
-        <v>2.05</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1978,16 +1876,16 @@
         <v>49</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>1.25</v>
       </c>
       <c r="D40">
-        <v>3.397058823529412</v>
+        <v>3.857142857142857</v>
       </c>
       <c r="E40">
-        <v>2.323529411764706</v>
+        <v>2.553571428571429</v>
       </c>
       <c r="F40">
         <v>2</v>
@@ -1999,13 +1897,13 @@
         <v>2.075</v>
       </c>
       <c r="I40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J40">
-        <v>3.125</v>
+        <v>3.833333333333333</v>
       </c>
       <c r="K40">
-        <v>2.3625</v>
+        <v>2.516666666666667</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2013,34 +1911,34 @@
         <v>50</v>
       </c>
       <c r="B41">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C41">
-        <v>1.805555555555556</v>
+        <v>2.159090909090909</v>
       </c>
       <c r="D41">
-        <v>3.717821782178218</v>
+        <v>3.855828220858896</v>
       </c>
       <c r="E41">
-        <v>2.761688668866887</v>
+        <v>3.007459564974902</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G41">
-        <v>3.583333333333333</v>
+        <v>4.285714285714286</v>
       </c>
       <c r="H41">
-        <v>2.391666666666667</v>
+        <v>2.842857142857143</v>
       </c>
       <c r="I41">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J41">
-        <v>3.166666666666667</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="K41">
-        <v>3.383333333333333</v>
+        <v>1.933333333333333</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2048,34 +1946,34 @@
         <v>51</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>1.25</v>
       </c>
       <c r="D42">
-        <v>3.214788732394366</v>
+        <v>3.433962264150944</v>
       </c>
       <c r="E42">
-        <v>2.232394366197183</v>
+        <v>2.341981132075472</v>
       </c>
       <c r="F42">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.1</v>
+        <v>2.75</v>
       </c>
       <c r="H42">
-        <v>2.05</v>
+        <v>1.575</v>
       </c>
       <c r="I42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J42">
-        <v>2.666666666666667</v>
+        <v>3.5</v>
       </c>
       <c r="K42">
-        <v>1.933333333333333</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2083,34 +1981,34 @@
         <v>52</v>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C43">
         <v>1.25</v>
       </c>
       <c r="D43">
-        <v>3.927480916030534</v>
+        <v>3.142857142857143</v>
       </c>
       <c r="E43">
-        <v>2.588740458015267</v>
+        <v>2.196428571428571</v>
       </c>
       <c r="F43">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G43">
-        <v>3.166666666666667</v>
+        <v>3.625</v>
       </c>
       <c r="H43">
-        <v>1.883333333333333</v>
+        <v>2.2125</v>
       </c>
       <c r="I43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J43">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="K43">
-        <v>2.35</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2118,34 +2016,28 @@
         <v>53</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>1.805555555555556</v>
+        <v>1.25</v>
       </c>
       <c r="D44">
-        <v>3.605603448275862</v>
+        <v>4.25</v>
       </c>
       <c r="E44">
-        <v>2.705579501915709</v>
+        <v>2.75</v>
       </c>
       <c r="F44">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G44">
-        <v>3.333333333333333</v>
+        <v>4.5</v>
       </c>
       <c r="H44">
-        <v>2.266666666666667</v>
+        <v>2.45</v>
       </c>
       <c r="I44">
-        <v>2</v>
-      </c>
-      <c r="J44">
-        <v>4.5</v>
-      </c>
-      <c r="K44">
-        <v>2.65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2153,34 +2045,34 @@
         <v>54</v>
       </c>
       <c r="B45">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>2.678571428571428</v>
+        <v>1.25</v>
       </c>
       <c r="D45">
-        <v>3.760378983634797</v>
+        <v>3.409090909090909</v>
       </c>
       <c r="E45">
-        <v>3.219475206103113</v>
+        <v>2.329545454545455</v>
       </c>
       <c r="F45">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>3.880952380952381</v>
+        <v>2.5</v>
       </c>
       <c r="H45">
-        <v>4.04047619047619</v>
+        <v>1.35</v>
       </c>
       <c r="I45">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J45">
-        <v>4.071428571428571</v>
+        <v>4</v>
       </c>
       <c r="K45">
-        <v>3.435714285714285</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2188,34 +2080,34 @@
         <v>55</v>
       </c>
       <c r="B46">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C46">
-        <v>1.75</v>
+        <v>1.25</v>
       </c>
       <c r="D46">
-        <v>3.847545219638243</v>
+        <v>3.566666666666667</v>
       </c>
       <c r="E46">
-        <v>2.798772609819121</v>
+        <v>2.408333333333333</v>
       </c>
       <c r="F46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G46">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="H46">
-        <v>2.55</v>
+        <v>2.95</v>
       </c>
       <c r="I46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J46">
-        <v>3.75</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="K46">
-        <v>2.275</v>
+        <v>1.766666666666667</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2223,34 +2115,34 @@
         <v>56</v>
       </c>
       <c r="B47">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C47">
-        <v>3.027777777777778</v>
+        <v>3.107142857142857</v>
       </c>
       <c r="D47">
-        <v>3.909684116861931</v>
+        <v>3.559424083769633</v>
       </c>
       <c r="E47">
-        <v>3.468730947319854</v>
+        <v>3.333283470456245</v>
       </c>
       <c r="F47">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G47">
-        <v>3.946428571428572</v>
+        <v>3.5</v>
       </c>
       <c r="H47">
-        <v>4.773214285714285</v>
+        <v>2.95</v>
       </c>
       <c r="I47">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J47">
-        <v>3.083333333333333</v>
+        <v>3.75</v>
       </c>
       <c r="K47">
-        <v>2.741666666666667</v>
+        <v>4.275</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2258,34 +2150,16 @@
         <v>57</v>
       </c>
       <c r="B48">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>3.25</v>
-      </c>
-      <c r="D48">
-        <v>3.555164835164835</v>
-      </c>
-      <c r="E48">
-        <v>3.402582417582417</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>10</v>
-      </c>
-      <c r="G48">
-        <v>3.5</v>
-      </c>
-      <c r="H48">
-        <v>2.75</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>7</v>
-      </c>
-      <c r="J48">
-        <v>3.571428571428572</v>
-      </c>
-      <c r="K48">
-        <v>3.185714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2293,34 +2167,34 @@
         <v>58</v>
       </c>
       <c r="B49">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C49">
-        <v>2.980769230769231</v>
+        <v>2.583333333333333</v>
       </c>
       <c r="D49">
-        <v>3.997177267595032</v>
+        <v>3.766937669376694</v>
       </c>
       <c r="E49">
-        <v>3.488973249182131</v>
+        <v>3.175135501355014</v>
       </c>
       <c r="F49">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G49">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="H49">
-        <v>3.275</v>
+        <v>2.45</v>
       </c>
       <c r="I49">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="J49">
-        <v>3.423076923076923</v>
+        <v>2.5</v>
       </c>
       <c r="K49">
-        <v>4.311538461538461</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2328,34 +2202,34 @@
         <v>59</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>1.25</v>
       </c>
       <c r="D50">
-        <v>3.977040816326531</v>
+        <v>3.397058823529412</v>
       </c>
       <c r="E50">
-        <v>2.613520408163265</v>
+        <v>2.323529411764706</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>4.166666666666667</v>
+        <v>3.75</v>
       </c>
       <c r="H50">
-        <v>2.383333333333333</v>
+        <v>2.075</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J50">
-        <v>3.75</v>
+        <v>3.125</v>
       </c>
       <c r="K50">
-        <v>2.275</v>
+        <v>2.3625</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2363,34 +2237,34 @@
         <v>60</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C51">
-        <v>2.916666666666667</v>
+        <v>1.805555555555556</v>
       </c>
       <c r="D51">
-        <v>4.486607142857143</v>
+        <v>3.717821782178218</v>
       </c>
       <c r="E51">
-        <v>3.701636904761905</v>
+        <v>2.761688668866887</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G51">
-        <v>4.5</v>
+        <v>3.583333333333333</v>
       </c>
       <c r="H51">
-        <v>2.45</v>
+        <v>2.391666666666667</v>
       </c>
       <c r="I51">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J51">
-        <v>4.5</v>
+        <v>3.166666666666667</v>
       </c>
       <c r="K51">
-        <v>2.65</v>
+        <v>3.383333333333333</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2398,34 +2272,34 @@
         <v>61</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C52">
         <v>1.25</v>
       </c>
       <c r="D52">
-        <v>3.87246963562753</v>
+        <v>3.20979020979021</v>
       </c>
       <c r="E52">
-        <v>2.561234817813765</v>
+        <v>2.229895104895105</v>
       </c>
       <c r="F52">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G52">
-        <v>3.863636363636364</v>
+        <v>3.1</v>
       </c>
       <c r="H52">
-        <v>3.031818181818182</v>
+        <v>2.05</v>
       </c>
       <c r="I52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J52">
-        <v>3.75</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="K52">
-        <v>2.275</v>
+        <v>1.933333333333333</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2433,34 +2307,34 @@
         <v>62</v>
       </c>
       <c r="B53">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C53">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="D53">
-        <v>3.714285714285714</v>
+        <v>3.927480916030534</v>
       </c>
       <c r="E53">
-        <v>3.107142857142857</v>
+        <v>2.588740458015267</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G53">
-        <v>2.5</v>
+        <v>3.166666666666667</v>
       </c>
       <c r="H53">
-        <v>1.35</v>
+        <v>1.883333333333333</v>
       </c>
       <c r="I53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J53">
-        <v>4.25</v>
+        <v>3.5</v>
       </c>
       <c r="K53">
-        <v>2.525</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2471,31 +2345,31 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>1.25</v>
+        <v>1.805555555555556</v>
       </c>
       <c r="D54">
-        <v>4.121104185218166</v>
+        <v>3.605603448275862</v>
       </c>
       <c r="E54">
-        <v>2.685552092609083</v>
+        <v>2.705579501915709</v>
       </c>
       <c r="F54">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="H54">
-        <v>2.9</v>
+        <v>2.266666666666667</v>
       </c>
       <c r="I54">
         <v>2</v>
       </c>
       <c r="J54">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="K54">
-        <v>1.15</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2503,34 +2377,28 @@
         <v>64</v>
       </c>
       <c r="B55">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>1.964285714285714</v>
-      </c>
-      <c r="D55">
-        <v>3.832309582309582</v>
-      </c>
-      <c r="E55">
-        <v>2.898297648297648</v>
+        <v>6.25</v>
       </c>
       <c r="F55">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="H55">
+        <v>2.6</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
         <v>4</v>
       </c>
-      <c r="H55">
-        <v>3.9</v>
-      </c>
-      <c r="I55">
-        <v>5</v>
-      </c>
-      <c r="J55">
-        <v>3.5</v>
-      </c>
       <c r="K55">
-        <v>2.75</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2538,34 +2406,34 @@
         <v>65</v>
       </c>
       <c r="B56">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C56">
-        <v>4.138888888888889</v>
+        <v>2.678571428571428</v>
       </c>
       <c r="D56">
-        <v>3.742219215155616</v>
+        <v>3.760375408989151</v>
       </c>
       <c r="E56">
-        <v>3.940554052022252</v>
+        <v>3.21947341878029</v>
       </c>
       <c r="F56">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G56">
-        <v>3.708333333333333</v>
+        <v>3.880952380952381</v>
       </c>
       <c r="H56">
-        <v>3.054166666666667</v>
+        <v>4.04047619047619</v>
       </c>
       <c r="I56">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J56">
-        <v>3.681818181818182</v>
+        <v>4.071428571428571</v>
       </c>
       <c r="K56">
-        <v>4.040909090909091</v>
+        <v>3.435714285714285</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2573,22 +2441,34 @@
         <v>66</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>3.847545219638243</v>
       </c>
       <c r="E57">
-        <v>3.125</v>
+        <v>2.798772609819121</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G57">
+        <v>3.5</v>
+      </c>
+      <c r="H57">
+        <v>2.55</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J57">
+        <v>3.75</v>
+      </c>
+      <c r="K57">
+        <v>2.275</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2596,34 +2476,34 @@
         <v>67</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C58">
-        <v>1.964285714285714</v>
+        <v>3.027777777777778</v>
       </c>
       <c r="D58">
-        <v>3.52212389380531</v>
+        <v>3.909684116861931</v>
       </c>
       <c r="E58">
-        <v>2.743204804045512</v>
+        <v>3.468730947319854</v>
       </c>
       <c r="F58">
+        <v>28</v>
+      </c>
+      <c r="G58">
+        <v>3.946428571428572</v>
+      </c>
+      <c r="H58">
+        <v>4.773214285714285</v>
+      </c>
+      <c r="I58">
         <v>6</v>
       </c>
-      <c r="G58">
-        <v>3.25</v>
-      </c>
-      <c r="H58">
-        <v>2.225</v>
-      </c>
-      <c r="I58">
-        <v>4</v>
-      </c>
       <c r="J58">
-        <v>4</v>
+        <v>3.083333333333333</v>
       </c>
       <c r="K58">
-        <v>2.8</v>
+        <v>2.741666666666667</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2631,34 +2511,16 @@
         <v>68</v>
       </c>
       <c r="B59">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>3.522727272727273</v>
-      </c>
-      <c r="D59">
-        <v>3.642351660315732</v>
-      </c>
-      <c r="E59">
-        <v>3.582539466521502</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>14</v>
-      </c>
-      <c r="G59">
-        <v>3.464285714285714</v>
-      </c>
-      <c r="H59">
-        <v>3.132142857142857</v>
+        <v>0</v>
       </c>
       <c r="I59">
-        <v>8</v>
-      </c>
-      <c r="J59">
-        <v>3.9375</v>
-      </c>
-      <c r="K59">
-        <v>3.56875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2666,34 +2528,34 @@
         <v>69</v>
       </c>
       <c r="B60">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C60">
-        <v>3.161764705882353</v>
+        <v>3.25</v>
       </c>
       <c r="D60">
-        <v>3.690427698574338</v>
+        <v>3.555164835164835</v>
       </c>
       <c r="E60">
-        <v>3.426096202228345</v>
+        <v>3.402582417582417</v>
       </c>
       <c r="F60">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G60">
-        <v>4.136363636363637</v>
+        <v>3.5</v>
       </c>
       <c r="H60">
-        <v>3.168181818181818</v>
+        <v>2.75</v>
       </c>
       <c r="I60">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J60">
-        <v>3.75</v>
+        <v>3.571428571428572</v>
       </c>
       <c r="K60">
-        <v>3.875</v>
+        <v>3.185714285714286</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2701,34 +2563,34 @@
         <v>70</v>
       </c>
       <c r="B61">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C61">
-        <v>2.083333333333333</v>
+        <v>2.980769230769231</v>
       </c>
       <c r="D61">
-        <v>4.124896608767576</v>
+        <v>3.998025944726452</v>
       </c>
       <c r="E61">
-        <v>3.104114971050455</v>
+        <v>3.489397587747842</v>
       </c>
       <c r="F61">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G61">
-        <v>3.8</v>
+        <v>3.785714285714286</v>
       </c>
       <c r="H61">
-        <v>2.9</v>
+        <v>3.292857142857143</v>
       </c>
       <c r="I61">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="J61">
-        <v>2.5</v>
+        <v>3.423076923076923</v>
       </c>
       <c r="K61">
-        <v>1.65</v>
+        <v>4.311538461538461</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2736,25 +2598,25 @@
         <v>71</v>
       </c>
       <c r="B62">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>3.25</v>
+        <v>1.25</v>
       </c>
       <c r="D62">
-        <v>3.909978880675818</v>
+        <v>3.977040816326531</v>
       </c>
       <c r="E62">
-        <v>3.579989440337909</v>
+        <v>2.613520408163265</v>
       </c>
       <c r="F62">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G62">
-        <v>3.541666666666667</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="H62">
-        <v>2.970833333333333</v>
+        <v>2.383333333333333</v>
       </c>
       <c r="I62">
         <v>2</v>
@@ -2771,34 +2633,34 @@
         <v>72</v>
       </c>
       <c r="B63">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>2.916666666666667</v>
       </c>
       <c r="D63">
-        <v>3.584249084249084</v>
+        <v>4.486607142857143</v>
       </c>
       <c r="E63">
-        <v>3.250457875457876</v>
+        <v>3.701636904761905</v>
       </c>
       <c r="F63">
         <v>2</v>
       </c>
       <c r="G63">
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="H63">
-        <v>2.575</v>
+        <v>2.45</v>
       </c>
       <c r="I63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J63">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="K63">
-        <v>2.1</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -2806,34 +2668,34 @@
         <v>73</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C64">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="D64">
-        <v>4.004237288135593</v>
+        <v>3.87246963562753</v>
       </c>
       <c r="E64">
-        <v>3.252118644067797</v>
+        <v>2.561234817813765</v>
       </c>
       <c r="F64">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G64">
-        <v>4</v>
+        <v>3.863636363636364</v>
       </c>
       <c r="H64">
-        <v>2.3</v>
+        <v>3.031818181818182</v>
       </c>
       <c r="I64">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J64">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="K64">
-        <v>3</v>
+        <v>2.275</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -2841,34 +2703,34 @@
         <v>74</v>
       </c>
       <c r="B65">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="C65">
-        <v>4.232456140350878</v>
+        <v>3.25</v>
       </c>
       <c r="D65">
-        <v>4.118747308189257</v>
+        <v>4.192737430167598</v>
       </c>
       <c r="E65">
-        <v>4.175601724270067</v>
+        <v>3.721368715083799</v>
       </c>
       <c r="F65">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G65">
-        <v>3.916666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="H65">
-        <v>4.358333333333333</v>
+        <v>1.35</v>
       </c>
       <c r="I65">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J65">
-        <v>4.21875</v>
+        <v>4.25</v>
       </c>
       <c r="K65">
-        <v>5.309375</v>
+        <v>2.525</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -2876,34 +2738,34 @@
         <v>75</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C66">
-        <v>2.678571428571428</v>
+        <v>1.25</v>
       </c>
       <c r="D66">
-        <v>4.012422360248447</v>
+        <v>4.121380846325167</v>
       </c>
       <c r="E66">
-        <v>3.345496894409938</v>
+        <v>2.685690423162583</v>
       </c>
       <c r="F66">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G66">
-        <v>2.833333333333333</v>
+        <v>4</v>
       </c>
       <c r="H66">
-        <v>2.016666666666667</v>
+        <v>2.9</v>
       </c>
       <c r="I66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J66">
-        <v>3.833333333333333</v>
+        <v>1.5</v>
       </c>
       <c r="K66">
-        <v>2.516666666666667</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -2911,34 +2773,34 @@
         <v>76</v>
       </c>
       <c r="B67">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C67">
-        <v>3.491379310344827</v>
+        <v>1.964285714285714</v>
       </c>
       <c r="D67">
-        <v>3.869124683366169</v>
+        <v>3.832309582309582</v>
       </c>
       <c r="E67">
-        <v>3.680251996855498</v>
+        <v>2.898297648297648</v>
       </c>
       <c r="F67">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G67">
-        <v>3.916666666666667</v>
+        <v>4</v>
       </c>
       <c r="H67">
-        <v>3.758333333333333</v>
+        <v>3.9</v>
       </c>
       <c r="I67">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J67">
-        <v>4.333333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="K67">
-        <v>3.366666666666666</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -2946,28 +2808,34 @@
         <v>77</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C68">
-        <v>1.25</v>
+        <v>4.138888888888889</v>
       </c>
       <c r="D68">
-        <v>3.678571428571428</v>
+        <v>3.74218089602705</v>
       </c>
       <c r="E68">
-        <v>2.464285714285714</v>
+        <v>3.940534892457969</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G68">
-        <v>3.5</v>
+        <v>3.708333333333333</v>
       </c>
       <c r="H68">
-        <v>1.85</v>
+        <v>3.054166666666667</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="J68">
+        <v>3.681818181818182</v>
+      </c>
+      <c r="K68">
+        <v>4.040909090909091</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -2975,34 +2843,22 @@
         <v>78</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>1.875</v>
+        <v>1.25</v>
       </c>
       <c r="D69">
-        <v>4.238738738738738</v>
+        <v>5</v>
       </c>
       <c r="E69">
-        <v>3.056869369369369</v>
+        <v>3.125</v>
       </c>
       <c r="F69">
-        <v>5</v>
-      </c>
-      <c r="G69">
-        <v>3.4</v>
-      </c>
-      <c r="H69">
-        <v>2.2</v>
+        <v>0</v>
       </c>
       <c r="I69">
-        <v>1</v>
-      </c>
-      <c r="J69">
-        <v>3.5</v>
-      </c>
-      <c r="K69">
-        <v>1.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3016,28 +2872,28 @@
         <v>1.964285714285714</v>
       </c>
       <c r="D70">
-        <v>3.939759036144578</v>
+        <v>3.52212389380531</v>
       </c>
       <c r="E70">
-        <v>2.952022375215146</v>
+        <v>2.743204804045512</v>
       </c>
       <c r="F70">
+        <v>6</v>
+      </c>
+      <c r="G70">
+        <v>3.25</v>
+      </c>
+      <c r="H70">
+        <v>2.225</v>
+      </c>
+      <c r="I70">
         <v>4</v>
       </c>
-      <c r="G70">
-        <v>4.5</v>
-      </c>
-      <c r="H70">
-        <v>2.65</v>
-      </c>
-      <c r="I70">
-        <v>6</v>
-      </c>
       <c r="J70">
-        <v>3.583333333333333</v>
+        <v>4</v>
       </c>
       <c r="K70">
-        <v>2.991666666666667</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -3045,34 +2901,34 @@
         <v>80</v>
       </c>
       <c r="B71">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C71">
-        <v>3.125</v>
+        <v>3.522727272727273</v>
       </c>
       <c r="D71">
-        <v>4.009595959595959</v>
+        <v>3.642351660315732</v>
       </c>
       <c r="E71">
-        <v>3.56729797979798</v>
+        <v>3.582539466521502</v>
       </c>
       <c r="F71">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G71">
-        <v>3.714285714285714</v>
+        <v>3.464285714285714</v>
       </c>
       <c r="H71">
-        <v>2.557142857142857</v>
+        <v>3.132142857142857</v>
       </c>
       <c r="I71">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J71">
-        <v>3.666666666666667</v>
+        <v>3.9375</v>
       </c>
       <c r="K71">
-        <v>2.433333333333333</v>
+        <v>3.56875</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -3080,34 +2936,34 @@
         <v>81</v>
       </c>
       <c r="B72">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C72">
+        <v>3.161764705882353</v>
+      </c>
+      <c r="D72">
+        <v>3.690577563865235</v>
+      </c>
+      <c r="E72">
+        <v>3.426171134873794</v>
+      </c>
+      <c r="F72">
+        <v>11</v>
+      </c>
+      <c r="G72">
+        <v>4.136363636363637</v>
+      </c>
+      <c r="H72">
+        <v>3.168181818181818</v>
+      </c>
+      <c r="I72">
+        <v>10</v>
+      </c>
+      <c r="J72">
         <v>3.75</v>
       </c>
-      <c r="D72">
-        <v>4.5</v>
-      </c>
-      <c r="E72">
-        <v>4.125</v>
-      </c>
-      <c r="F72">
-        <v>5</v>
-      </c>
-      <c r="G72">
-        <v>3.7</v>
-      </c>
-      <c r="H72">
-        <v>2.35</v>
-      </c>
-      <c r="I72">
-        <v>2</v>
-      </c>
-      <c r="J72">
-        <v>3.25</v>
-      </c>
       <c r="K72">
-        <v>2.025</v>
+        <v>3.875</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -3115,34 +2971,34 @@
         <v>82</v>
       </c>
       <c r="B73">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>3.206521739130435</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="D73">
-        <v>3.707438281500481</v>
+        <v>4.124896608767576</v>
       </c>
       <c r="E73">
-        <v>3.456980010315458</v>
+        <v>3.104114971050455</v>
       </c>
       <c r="F73">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G73">
-        <v>3.681818181818182</v>
+        <v>3.8</v>
       </c>
       <c r="H73">
-        <v>2.940909090909091</v>
+        <v>2.9</v>
       </c>
       <c r="I73">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J73">
-        <v>3.7</v>
+        <v>2.5</v>
       </c>
       <c r="K73">
-        <v>2.85</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -3150,34 +3006,34 @@
         <v>83</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C74">
-        <v>2.25</v>
+        <v>3.25</v>
       </c>
       <c r="D74">
-        <v>4.102424242424243</v>
+        <v>3.910026385224274</v>
       </c>
       <c r="E74">
-        <v>3.176212121212121</v>
+        <v>3.580013192612137</v>
       </c>
       <c r="F74">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G74">
-        <v>4.166666666666667</v>
+        <v>3.541666666666667</v>
       </c>
       <c r="H74">
-        <v>2.383333333333333</v>
+        <v>2.970833333333333</v>
       </c>
       <c r="I74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J74">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="K74">
-        <v>2.7</v>
+        <v>2.275</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -3185,34 +3041,34 @@
         <v>84</v>
       </c>
       <c r="B75">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <v>3.125</v>
+        <v>2.916666666666667</v>
       </c>
       <c r="D75">
-        <v>3.548387096774194</v>
+        <v>3.584249084249084</v>
       </c>
       <c r="E75">
-        <v>3.336693548387097</v>
+        <v>3.250457875457876</v>
       </c>
       <c r="F75">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G75">
-        <v>3.166666666666667</v>
+        <v>4.75</v>
       </c>
       <c r="H75">
-        <v>2.483333333333333</v>
+        <v>2.575</v>
       </c>
       <c r="I75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J75">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="K75">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -3220,34 +3076,34 @@
         <v>85</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C76">
-        <v>2.678571428571428</v>
+        <v>2.5</v>
       </c>
       <c r="D76">
-        <v>3.943306010928962</v>
+        <v>4.004237288135593</v>
       </c>
       <c r="E76">
-        <v>3.310938719750195</v>
+        <v>3.252118644067797</v>
       </c>
       <c r="F76">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G76">
-        <v>3.888888888888889</v>
+        <v>4</v>
       </c>
       <c r="H76">
-        <v>2.844444444444445</v>
+        <v>2.3</v>
       </c>
       <c r="I76">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J76">
-        <v>3.571428571428572</v>
+        <v>4</v>
       </c>
       <c r="K76">
-        <v>3.185714285714286</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -3255,34 +3111,34 @@
         <v>86</v>
       </c>
       <c r="B77">
+        <v>57</v>
+      </c>
+      <c r="C77">
+        <v>4.232456140350878</v>
+      </c>
+      <c r="D77">
+        <v>4.118764991696906</v>
+      </c>
+      <c r="E77">
+        <v>4.175610566023892</v>
+      </c>
+      <c r="F77">
         <v>24</v>
       </c>
-      <c r="C77">
-        <v>2.083333333333333</v>
-      </c>
-      <c r="D77">
-        <v>3.421862011637573</v>
-      </c>
-      <c r="E77">
-        <v>2.752597672485453</v>
-      </c>
-      <c r="F77">
-        <v>12</v>
-      </c>
       <c r="G77">
-        <v>3.5</v>
+        <v>3.916666666666667</v>
       </c>
       <c r="H77">
-        <v>2.95</v>
+        <v>4.358333333333333</v>
       </c>
       <c r="I77">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J77">
-        <v>3.833333333333333</v>
+        <v>4.21875</v>
       </c>
       <c r="K77">
-        <v>3.116666666666667</v>
+        <v>5.309375</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -3290,34 +3146,34 @@
         <v>87</v>
       </c>
       <c r="B78">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="C78">
-        <v>2.591463414634147</v>
+        <v>2.678571428571428</v>
       </c>
       <c r="D78">
-        <v>3.576799485861183</v>
+        <v>4.012422360248447</v>
       </c>
       <c r="E78">
-        <v>3.084131450247665</v>
+        <v>3.345496894409938</v>
       </c>
       <c r="F78">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G78">
-        <v>3.535714285714286</v>
+        <v>2.833333333333333</v>
       </c>
       <c r="H78">
-        <v>3.167857142857143</v>
+        <v>2.016666666666667</v>
       </c>
       <c r="I78">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="J78">
-        <v>3.2</v>
+        <v>3.833333333333333</v>
       </c>
       <c r="K78">
-        <v>4.6</v>
+        <v>2.516666666666667</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -3325,34 +3181,34 @@
         <v>88</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C79">
-        <v>3.014705882352941</v>
+        <v>3.491379310344827</v>
       </c>
       <c r="D79">
-        <v>3.654159132007233</v>
+        <v>3.86937570303712</v>
       </c>
       <c r="E79">
-        <v>3.334432507180087</v>
+        <v>3.680377506690974</v>
       </c>
       <c r="F79">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G79">
-        <v>3.375</v>
+        <v>3.916666666666667</v>
       </c>
       <c r="H79">
-        <v>2.4875</v>
+        <v>3.758333333333333</v>
       </c>
       <c r="I79">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J79">
-        <v>3.2</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="K79">
-        <v>2.6</v>
+        <v>3.366666666666666</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -3360,34 +3216,28 @@
         <v>89</v>
       </c>
       <c r="B80">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C80">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="D80">
-        <v>3.791907514450867</v>
+        <v>3.678571428571428</v>
       </c>
       <c r="E80">
-        <v>3.145953757225433</v>
+        <v>2.464285714285714</v>
       </c>
       <c r="F80">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G80">
         <v>3.5</v>
       </c>
       <c r="H80">
-        <v>2.25</v>
+        <v>1.85</v>
       </c>
       <c r="I80">
-        <v>1</v>
-      </c>
-      <c r="J80">
-        <v>4</v>
-      </c>
-      <c r="K80">
-        <v>2.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -3395,34 +3245,34 @@
         <v>90</v>
       </c>
       <c r="B81">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C81">
-        <v>1.964285714285714</v>
+        <v>1.875</v>
       </c>
       <c r="D81">
-        <v>3.183011049723757</v>
+        <v>4.238738738738738</v>
       </c>
       <c r="E81">
-        <v>2.573648382004736</v>
+        <v>3.056869369369369</v>
       </c>
       <c r="F81">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G81">
-        <v>2.875</v>
+        <v>3.4</v>
       </c>
       <c r="H81">
-        <v>1.8375</v>
+        <v>2.2</v>
       </c>
       <c r="I81">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J81">
-        <v>4.166666666666667</v>
+        <v>3.5</v>
       </c>
       <c r="K81">
-        <v>3.283333333333333</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -3430,28 +3280,34 @@
         <v>91</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C82">
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="D82">
-        <v>4.5</v>
+        <v>3.872448979591837</v>
       </c>
       <c r="E82">
-        <v>2.875</v>
+        <v>3.186224489795919</v>
       </c>
       <c r="F82">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G82">
         <v>4.5</v>
       </c>
       <c r="H82">
-        <v>2.35</v>
+        <v>2.65</v>
       </c>
       <c r="I82">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="J82">
+        <v>3.583333333333333</v>
+      </c>
+      <c r="K82">
+        <v>2.991666666666667</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -3459,28 +3315,34 @@
         <v>92</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C83">
-        <v>1.25</v>
+        <v>3.125</v>
       </c>
       <c r="D83">
-        <v>4.569767441860465</v>
+        <v>4.009600808489136</v>
       </c>
       <c r="E83">
-        <v>2.909883720930233</v>
+        <v>3.567300404244568</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G83">
+        <v>3.714285714285714</v>
+      </c>
+      <c r="H83">
+        <v>2.557142857142857</v>
       </c>
       <c r="I83">
         <v>3</v>
       </c>
       <c r="J83">
-        <v>3.333333333333333</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="K83">
-        <v>2.266666666666667</v>
+        <v>2.433333333333333</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -3488,34 +3350,34 @@
         <v>93</v>
       </c>
       <c r="B84">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C84">
-        <v>1.875</v>
+        <v>3.75</v>
       </c>
       <c r="D84">
-        <v>3.55</v>
+        <v>4.5</v>
       </c>
       <c r="E84">
-        <v>2.7125</v>
+        <v>4.125</v>
       </c>
       <c r="F84">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G84">
-        <v>3.666666666666667</v>
+        <v>3.7</v>
       </c>
       <c r="H84">
-        <v>2.133333333333333</v>
+        <v>2.35</v>
       </c>
       <c r="I84">
         <v>2</v>
       </c>
       <c r="J84">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="K84">
-        <v>1.775</v>
+        <v>2.025</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -3523,34 +3385,34 @@
         <v>94</v>
       </c>
       <c r="B85">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C85">
-        <v>2.083333333333333</v>
+        <v>3.206521739130435</v>
       </c>
       <c r="D85">
-        <v>3.611111111111111</v>
+        <v>3.707438281500481</v>
       </c>
       <c r="E85">
-        <v>2.847222222222222</v>
+        <v>3.456980010315458</v>
       </c>
       <c r="F85">
+        <v>11</v>
+      </c>
+      <c r="G85">
+        <v>3.681818181818182</v>
+      </c>
+      <c r="H85">
+        <v>2.940909090909091</v>
+      </c>
+      <c r="I85">
         <v>5</v>
       </c>
-      <c r="G85">
-        <v>2.9</v>
-      </c>
-      <c r="H85">
-        <v>1.95</v>
-      </c>
-      <c r="I85">
-        <v>3</v>
-      </c>
       <c r="J85">
-        <v>4.166666666666667</v>
+        <v>3.7</v>
       </c>
       <c r="K85">
-        <v>2.683333333333334</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -3558,28 +3420,34 @@
         <v>95</v>
       </c>
       <c r="B86">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C86">
-        <v>1.25</v>
+        <v>2.25</v>
       </c>
       <c r="D86">
-        <v>3.513986013986014</v>
+        <v>4.102424242424243</v>
       </c>
       <c r="E86">
-        <v>2.381993006993007</v>
+        <v>3.176212121212121</v>
       </c>
       <c r="F86">
         <v>3</v>
       </c>
       <c r="G86">
-        <v>3.5</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="H86">
-        <v>2.05</v>
+        <v>2.383333333333333</v>
       </c>
       <c r="I86">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>5</v>
+      </c>
+      <c r="K86">
+        <v>2.7</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -3587,22 +3455,34 @@
         <v>96</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C87">
-        <v>2.5</v>
+        <v>3.125</v>
       </c>
       <c r="D87">
-        <v>4.322222222222222</v>
+        <v>3.548387096774194</v>
       </c>
       <c r="E87">
-        <v>3.411111111111111</v>
+        <v>3.336693548387097</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G87">
+        <v>3.166666666666667</v>
+      </c>
+      <c r="H87">
+        <v>2.483333333333333</v>
       </c>
       <c r="I87">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>3.5</v>
+      </c>
+      <c r="K87">
+        <v>1.95</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -3610,28 +3490,34 @@
         <v>97</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C88">
-        <v>1.25</v>
+        <v>2.678571428571428</v>
       </c>
       <c r="D88">
-        <v>4.5</v>
+        <v>3.944065484311051</v>
       </c>
       <c r="E88">
-        <v>2.875</v>
+        <v>3.311318456441239</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G88">
-        <v>4</v>
+        <v>3.888888888888889</v>
       </c>
       <c r="H88">
-        <v>2.1</v>
+        <v>2.844444444444445</v>
       </c>
       <c r="I88">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="J88">
+        <v>3.571428571428572</v>
+      </c>
+      <c r="K88">
+        <v>3.185714285714286</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -3639,34 +3525,34 @@
         <v>98</v>
       </c>
       <c r="B89">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C89">
-        <v>1.607142857142857</v>
+        <v>2.083333333333333</v>
       </c>
       <c r="D89">
-        <v>3.08273381294964</v>
+        <v>3.421862011637573</v>
       </c>
       <c r="E89">
-        <v>2.344938335046248</v>
+        <v>2.752597672485453</v>
       </c>
       <c r="F89">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G89">
-        <v>3.4375</v>
+        <v>3.5</v>
       </c>
       <c r="H89">
-        <v>2.51875</v>
+        <v>2.95</v>
       </c>
       <c r="I89">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J89">
-        <v>3.666666666666667</v>
+        <v>3.833333333333333</v>
       </c>
       <c r="K89">
-        <v>2.433333333333333</v>
+        <v>3.116666666666667</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -3674,28 +3560,34 @@
         <v>99</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C90">
-        <v>1.25</v>
+        <v>2.591463414634147</v>
       </c>
       <c r="D90">
-        <v>4.5</v>
+        <v>3.576502732240437</v>
       </c>
       <c r="E90">
-        <v>2.875</v>
+        <v>3.083983073437292</v>
       </c>
       <c r="F90">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G90">
-        <v>4.25</v>
+        <v>3.535714285714286</v>
       </c>
       <c r="H90">
-        <v>2.325</v>
+        <v>3.167857142857143</v>
       </c>
       <c r="I90">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="J90">
+        <v>3.2</v>
+      </c>
+      <c r="K90">
+        <v>4.6</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -3703,34 +3595,34 @@
         <v>100</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C91">
-        <v>1.25</v>
+        <v>3.014705882352941</v>
       </c>
       <c r="D91">
-        <v>4.25984251968504</v>
+        <v>3.654159132007233</v>
       </c>
       <c r="E91">
-        <v>2.75492125984252</v>
+        <v>3.334432507180087</v>
       </c>
       <c r="F91">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G91">
-        <v>3.833333333333333</v>
+        <v>3.375</v>
       </c>
       <c r="H91">
-        <v>2.216666666666667</v>
+        <v>2.4875</v>
       </c>
       <c r="I91">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J91">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="K91">
-        <v>1.7</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -3738,28 +3630,34 @@
         <v>101</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C92">
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="D92">
-        <v>2.5</v>
+        <v>3.791907514450867</v>
       </c>
       <c r="E92">
-        <v>1.875</v>
+        <v>3.145953757225433</v>
       </c>
       <c r="F92">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G92">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="H92">
-        <v>1.35</v>
+        <v>2.25</v>
       </c>
       <c r="I92">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>4</v>
+      </c>
+      <c r="K92">
+        <v>2.2</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -3767,34 +3665,34 @@
         <v>102</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C93">
-        <v>2.916666666666667</v>
+        <v>1.964285714285714</v>
       </c>
       <c r="D93">
-        <v>4</v>
+        <v>3.183011049723757</v>
       </c>
       <c r="E93">
-        <v>3.458333333333333</v>
+        <v>2.573648382004736</v>
       </c>
       <c r="F93">
         <v>4</v>
       </c>
       <c r="G93">
-        <v>3.375</v>
+        <v>2.875</v>
       </c>
       <c r="H93">
-        <v>2.0875</v>
+        <v>1.8375</v>
       </c>
       <c r="I93">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J93">
-        <v>3.5</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="K93">
-        <v>2.75</v>
+        <v>3.283333333333333</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -3802,34 +3700,16 @@
         <v>103</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C94">
-        <v>1.25</v>
-      </c>
-      <c r="D94">
-        <v>4.119834710743802</v>
-      </c>
-      <c r="E94">
-        <v>2.684917355371901</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>5</v>
-      </c>
-      <c r="G94">
-        <v>3.4</v>
-      </c>
-      <c r="H94">
-        <v>2.2</v>
+        <v>0</v>
       </c>
       <c r="I94">
-        <v>1</v>
-      </c>
-      <c r="J94">
-        <v>4.5</v>
-      </c>
-      <c r="K94">
-        <v>2.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -3837,25 +3717,13 @@
         <v>104</v>
       </c>
       <c r="B95">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>1.25</v>
-      </c>
-      <c r="D95">
-        <v>4.5</v>
-      </c>
-      <c r="E95">
-        <v>2.875</v>
+        <v>0</v>
       </c>
       <c r="F95">
-        <v>2</v>
-      </c>
-      <c r="G95">
-        <v>4.25</v>
-      </c>
-      <c r="H95">
-        <v>2.325</v>
+        <v>0</v>
       </c>
       <c r="I95">
         <v>0</v>
@@ -3866,34 +3734,16 @@
         <v>105</v>
       </c>
       <c r="B96">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C96">
-        <v>2.019230769230769</v>
-      </c>
-      <c r="D96">
-        <v>3.112094395280236</v>
-      </c>
-      <c r="E96">
-        <v>2.565662582255503</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>6</v>
-      </c>
-      <c r="G96">
-        <v>3.416666666666667</v>
-      </c>
-      <c r="H96">
-        <v>2.308333333333333</v>
+        <v>0</v>
       </c>
       <c r="I96">
-        <v>6</v>
-      </c>
-      <c r="J96">
-        <v>2.75</v>
-      </c>
-      <c r="K96">
-        <v>2.575</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -3901,34 +3751,22 @@
         <v>106</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C97">
-        <v>1.25</v>
-      </c>
-      <c r="D97">
-        <v>3.620481927710844</v>
-      </c>
-      <c r="E97">
-        <v>2.435240963855422</v>
+        <v>6.25</v>
       </c>
       <c r="F97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G97">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="H97">
-        <v>2.075</v>
+        <v>2.6</v>
       </c>
       <c r="I97">
-        <v>1</v>
-      </c>
-      <c r="J97">
-        <v>3</v>
-      </c>
-      <c r="K97">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -3936,34 +3774,28 @@
         <v>107</v>
       </c>
       <c r="B98">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C98">
-        <v>2.25</v>
+        <v>1.25</v>
       </c>
       <c r="D98">
-        <v>3.503894839337877</v>
+        <v>4.5</v>
       </c>
       <c r="E98">
-        <v>2.876947419668939</v>
+        <v>2.875</v>
       </c>
       <c r="F98">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G98">
-        <v>3.545454545454545</v>
+        <v>4.5</v>
       </c>
       <c r="H98">
-        <v>2.872727272727273</v>
+        <v>2.35</v>
       </c>
       <c r="I98">
-        <v>12</v>
-      </c>
-      <c r="J98">
-        <v>3.833333333333333</v>
-      </c>
-      <c r="K98">
-        <v>4.316666666666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -3977,21 +3809,533 @@
         <v>1.25</v>
       </c>
       <c r="D99">
+        <v>4.569767441860465</v>
+      </c>
+      <c r="E99">
+        <v>2.909883720930233</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>3</v>
+      </c>
+      <c r="J99">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="K99">
+        <v>2.266666666666667</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100">
+        <v>8</v>
+      </c>
+      <c r="C100">
+        <v>1.875</v>
+      </c>
+      <c r="D100">
+        <v>3.55</v>
+      </c>
+      <c r="E100">
+        <v>2.7125</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>3.666666666666667</v>
+      </c>
+      <c r="H100">
+        <v>2.133333333333333</v>
+      </c>
+      <c r="I100">
+        <v>2</v>
+      </c>
+      <c r="J100">
+        <v>2.75</v>
+      </c>
+      <c r="K100">
+        <v>1.775</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B101">
+        <v>12</v>
+      </c>
+      <c r="C101">
+        <v>2.083333333333333</v>
+      </c>
+      <c r="D101">
+        <v>3.611111111111111</v>
+      </c>
+      <c r="E101">
+        <v>2.847222222222222</v>
+      </c>
+      <c r="F101">
+        <v>5</v>
+      </c>
+      <c r="G101">
+        <v>2.9</v>
+      </c>
+      <c r="H101">
+        <v>1.95</v>
+      </c>
+      <c r="I101">
+        <v>3</v>
+      </c>
+      <c r="J101">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="K101">
+        <v>2.683333333333334</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>1.25</v>
+      </c>
+      <c r="D102">
+        <v>3.513986013986014</v>
+      </c>
+      <c r="E102">
+        <v>2.381993006993007</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <v>3.5</v>
+      </c>
+      <c r="H102">
+        <v>2.05</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B103">
+        <v>4</v>
+      </c>
+      <c r="C103">
+        <v>2.5</v>
+      </c>
+      <c r="D103">
+        <v>4.322222222222222</v>
+      </c>
+      <c r="E103">
+        <v>3.411111111111111</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>1.25</v>
+      </c>
+      <c r="D104">
+        <v>4.5</v>
+      </c>
+      <c r="E104">
+        <v>2.875</v>
+      </c>
+      <c r="F104">
+        <v>1</v>
+      </c>
+      <c r="G104">
+        <v>4</v>
+      </c>
+      <c r="H104">
+        <v>2.1</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105">
+        <v>14</v>
+      </c>
+      <c r="C105">
+        <v>1.607142857142857</v>
+      </c>
+      <c r="D105">
+        <v>3.08273381294964</v>
+      </c>
+      <c r="E105">
+        <v>2.344938335046248</v>
+      </c>
+      <c r="F105">
+        <v>8</v>
+      </c>
+      <c r="G105">
+        <v>3.4375</v>
+      </c>
+      <c r="H105">
+        <v>2.51875</v>
+      </c>
+      <c r="I105">
+        <v>3</v>
+      </c>
+      <c r="J105">
+        <v>3.666666666666667</v>
+      </c>
+      <c r="K105">
+        <v>2.433333333333333</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>1.25</v>
+      </c>
+      <c r="D106">
+        <v>4.5</v>
+      </c>
+      <c r="E106">
+        <v>2.875</v>
+      </c>
+      <c r="F106">
+        <v>2</v>
+      </c>
+      <c r="G106">
+        <v>4.25</v>
+      </c>
+      <c r="H106">
+        <v>2.325</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B107">
+        <v>4</v>
+      </c>
+      <c r="C107">
+        <v>1.25</v>
+      </c>
+      <c r="D107">
+        <v>4.25984251968504</v>
+      </c>
+      <c r="E107">
+        <v>2.75492125984252</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107">
+        <v>3.833333333333333</v>
+      </c>
+      <c r="H107">
+        <v>2.216666666666667</v>
+      </c>
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <v>3</v>
+      </c>
+      <c r="K107">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>1.25</v>
+      </c>
+      <c r="D108">
+        <v>2.5</v>
+      </c>
+      <c r="E108">
+        <v>1.875</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="G108">
+        <v>2.5</v>
+      </c>
+      <c r="H108">
+        <v>1.35</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+      <c r="C109">
+        <v>2.916666666666667</v>
+      </c>
+      <c r="D109">
+        <v>4</v>
+      </c>
+      <c r="E109">
+        <v>3.458333333333333</v>
+      </c>
+      <c r="F109">
+        <v>4</v>
+      </c>
+      <c r="G109">
+        <v>3.375</v>
+      </c>
+      <c r="H109">
+        <v>2.0875</v>
+      </c>
+      <c r="I109">
+        <v>5</v>
+      </c>
+      <c r="J109">
+        <v>3.5</v>
+      </c>
+      <c r="K109">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="A110" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B110">
+        <v>4</v>
+      </c>
+      <c r="C110">
+        <v>1.25</v>
+      </c>
+      <c r="D110">
+        <v>4.118131868131868</v>
+      </c>
+      <c r="E110">
+        <v>2.684065934065934</v>
+      </c>
+      <c r="F110">
+        <v>5</v>
+      </c>
+      <c r="G110">
+        <v>3.4</v>
+      </c>
+      <c r="H110">
+        <v>2.2</v>
+      </c>
+      <c r="I110">
+        <v>1</v>
+      </c>
+      <c r="J110">
+        <v>4.5</v>
+      </c>
+      <c r="K110">
+        <v>2.45</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="A111" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="C111">
+        <v>1.25</v>
+      </c>
+      <c r="D111">
+        <v>4.5</v>
+      </c>
+      <c r="E111">
+        <v>2.875</v>
+      </c>
+      <c r="F111">
+        <v>2</v>
+      </c>
+      <c r="G111">
+        <v>4.25</v>
+      </c>
+      <c r="H111">
+        <v>2.325</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
+      <c r="A112" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B112">
+        <v>13</v>
+      </c>
+      <c r="C112">
+        <v>2.019230769230769</v>
+      </c>
+      <c r="D112">
+        <v>3.112094395280236</v>
+      </c>
+      <c r="E112">
+        <v>2.565662582255503</v>
+      </c>
+      <c r="F112">
+        <v>6</v>
+      </c>
+      <c r="G112">
+        <v>3.416666666666667</v>
+      </c>
+      <c r="H112">
+        <v>2.308333333333333</v>
+      </c>
+      <c r="I112">
+        <v>6</v>
+      </c>
+      <c r="J112">
+        <v>2.75</v>
+      </c>
+      <c r="K112">
+        <v>2.575</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
+      <c r="A113" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>1.25</v>
+      </c>
+      <c r="D113">
+        <v>3.620481927710844</v>
+      </c>
+      <c r="E113">
+        <v>2.435240963855422</v>
+      </c>
+      <c r="F113">
+        <v>2</v>
+      </c>
+      <c r="G113">
+        <v>3.75</v>
+      </c>
+      <c r="H113">
+        <v>2.075</v>
+      </c>
+      <c r="I113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>3</v>
+      </c>
+      <c r="K113">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
+      <c r="A114" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B114">
+        <v>15</v>
+      </c>
+      <c r="C114">
+        <v>2.25</v>
+      </c>
+      <c r="D114">
+        <v>3.503894839337877</v>
+      </c>
+      <c r="E114">
+        <v>2.876947419668939</v>
+      </c>
+      <c r="F114">
+        <v>11</v>
+      </c>
+      <c r="G114">
+        <v>3.545454545454545</v>
+      </c>
+      <c r="H114">
+        <v>2.872727272727273</v>
+      </c>
+      <c r="I114">
+        <v>12</v>
+      </c>
+      <c r="J114">
+        <v>3.833333333333333</v>
+      </c>
+      <c r="K114">
+        <v>4.316666666666666</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
+      <c r="A115" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>1.25</v>
+      </c>
+      <c r="D115">
         <v>4.078947368421052</v>
       </c>
-      <c r="E99">
+      <c r="E115">
         <v>2.664473684210526</v>
       </c>
-      <c r="F99">
-        <v>1</v>
-      </c>
-      <c r="G99">
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115">
         <v>2.5</v>
       </c>
-      <c r="H99">
+      <c r="H115">
         <v>1.35</v>
       </c>
-      <c r="I99">
+      <c r="I115">
         <v>0</v>
       </c>
     </row>

</xml_diff>